<commit_message>
ADD: New logic of daily use and prod plan read data
</commit_message>
<xml_diff>
--- a/public/prod_plan/DailyUseTest1.xlsx
+++ b/public/prod_plan/DailyUseTest1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Telkom University\- Matkul sem 5 -\Magang\scope\be-scope\public\prod_plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Telkom University\- Matkul sem 5 -\Magang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8061B6AE-5677-4DF8-A642-06186CFD044E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B08D756-EAC6-48C5-B791-6966BD5054FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DAB1D4BE-B0C1-4C13-98F9-4212A95D167C}"/>
   </bookViews>
@@ -36,18 +36,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>partno</t>
   </si>
   <si>
-    <t>daily_use</t>
+    <t>year</t>
   </si>
   <si>
-    <t>plan_date</t>
+    <t>period</t>
   </si>
   <si>
-    <t>RL1EX045133MERD20000</t>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>DAILY USE</t>
+  </si>
+  <si>
+    <t>AL1LM0300DXL50G00000</t>
+  </si>
+  <si>
+    <t>AL3KB0KARBOXSIKU5000</t>
   </si>
 </sst>
 </file>
@@ -116,16 +125,16 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -462,117 +471,685 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD6BD1A7-9674-4A48-858C-A767ED342D2D}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A2:AI17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5:AI5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.54296875" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" customWidth="1"/>
+    <col min="1" max="1" width="4.36328125" customWidth="1"/>
+    <col min="2" max="2" width="27.54296875" customWidth="1"/>
     <col min="3" max="3" width="14.7265625" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>2</v>
+      </c>
+      <c r="G3" s="3">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
-        <v>2000</v>
-      </c>
-      <c r="C2" s="3">
-        <v>46001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="H3" s="3">
+        <v>4</v>
+      </c>
+      <c r="I3" s="3">
+        <v>5</v>
+      </c>
+      <c r="J3" s="3">
+        <v>6</v>
+      </c>
+      <c r="K3" s="3">
+        <v>7</v>
+      </c>
+      <c r="L3" s="3">
+        <v>8</v>
+      </c>
+      <c r="M3" s="3">
+        <v>9</v>
+      </c>
+      <c r="N3" s="3">
+        <v>10</v>
+      </c>
+      <c r="O3" s="3">
+        <v>11</v>
+      </c>
+      <c r="P3" s="3">
+        <v>12</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>13</v>
+      </c>
+      <c r="R3" s="3">
+        <v>14</v>
+      </c>
+      <c r="S3" s="3">
+        <v>15</v>
+      </c>
+      <c r="T3" s="3">
+        <v>16</v>
+      </c>
+      <c r="U3" s="3">
+        <v>17</v>
+      </c>
+      <c r="V3" s="3">
+        <v>18</v>
+      </c>
+      <c r="W3" s="3">
+        <v>19</v>
+      </c>
+      <c r="X3" s="3">
+        <v>20</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>21</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>22</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>23</v>
+      </c>
+      <c r="AB3" s="3">
+        <v>24</v>
+      </c>
+      <c r="AC3" s="3">
+        <v>25</v>
+      </c>
+      <c r="AD3" s="3">
+        <v>26</v>
+      </c>
+      <c r="AE3" s="3">
+        <v>27</v>
+      </c>
+      <c r="AF3" s="3">
+        <v>28</v>
+      </c>
+      <c r="AG3" s="3">
+        <v>29</v>
+      </c>
+      <c r="AH3" s="3">
+        <v>30</v>
+      </c>
+      <c r="AI3" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2026</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>300</v>
+      </c>
+      <c r="F4" s="3">
+        <v>300</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
+        <v>400</v>
+      </c>
+      <c r="I4" s="3">
+        <v>500</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0</v>
+      </c>
+      <c r="N4" s="3">
+        <v>0</v>
+      </c>
+      <c r="O4" s="3">
+        <v>0</v>
+      </c>
+      <c r="P4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>0</v>
+      </c>
+      <c r="R4" s="3">
+        <v>0</v>
+      </c>
+      <c r="S4" s="3">
+        <v>0</v>
+      </c>
+      <c r="T4" s="3">
+        <v>0</v>
+      </c>
+      <c r="U4" s="3">
+        <v>0</v>
+      </c>
+      <c r="V4" s="3">
+        <v>0</v>
+      </c>
+      <c r="W4" s="3">
+        <v>0</v>
+      </c>
+      <c r="X4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A5" s="3">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2026</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
+        <v>300</v>
+      </c>
+      <c r="F5" s="3">
+        <v>400</v>
+      </c>
+      <c r="G5" s="3">
+        <v>700</v>
+      </c>
+      <c r="H5" s="3">
+        <v>900</v>
+      </c>
+      <c r="I5" s="3">
+        <v>100</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0</v>
+      </c>
+      <c r="P5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>0</v>
+      </c>
+      <c r="R5" s="3">
+        <v>0</v>
+      </c>
+      <c r="S5" s="3">
+        <v>0</v>
+      </c>
+      <c r="T5" s="3">
+        <v>0</v>
+      </c>
+      <c r="U5" s="3">
+        <v>0</v>
+      </c>
+      <c r="V5" s="3">
+        <v>0</v>
+      </c>
+      <c r="W5" s="3">
+        <v>0</v>
+      </c>
+      <c r="X5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A6" s="3">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="3"/>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A7" s="3">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="3"/>
+      <c r="AH7" s="3"/>
+      <c r="AI7" s="3"/>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A8" s="3">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3"/>
+      <c r="AF8" s="3"/>
+      <c r="AG8" s="3"/>
+      <c r="AH8" s="3"/>
+      <c r="AI8" s="3"/>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A9" s="3">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3"/>
+      <c r="AF9" s="3"/>
+      <c r="AG9" s="3"/>
+      <c r="AH9" s="3"/>
+      <c r="AI9" s="3"/>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A10" s="3">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="3"/>
+      <c r="AE10" s="3"/>
+      <c r="AF10" s="3"/>
+      <c r="AG10" s="3"/>
+      <c r="AH10" s="3"/>
+      <c r="AI10" s="3"/>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A11" s="3">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="3"/>
+      <c r="AE11" s="3"/>
+      <c r="AF11" s="3"/>
+      <c r="AG11" s="3"/>
+      <c r="AH11" s="3"/>
+      <c r="AI11" s="3"/>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A12" s="3">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="3"/>
+      <c r="AE12" s="3"/>
+      <c r="AF12" s="3"/>
+      <c r="AG12" s="3"/>
+      <c r="AH12" s="3"/>
+      <c r="AI12" s="3"/>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A13" s="3">
+        <v>10</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
+      <c r="AA13" s="3"/>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="3"/>
+      <c r="AE13" s="3"/>
+      <c r="AF13" s="3"/>
+      <c r="AG13" s="3"/>
+      <c r="AH13" s="3"/>
+      <c r="AI13" s="3"/>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:D2"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ADD: New method od logistics daily shipment and fix new logic of daily use
</commit_message>
<xml_diff>
--- a/public/prod_plan/DailyUseTest1.xlsx
+++ b/public/prod_plan/DailyUseTest1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Telkom University\- Matkul sem 5 -\Magang\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Telkom University\- Matkul sem 5 -\Magang\scope\be-scope\public\prod_plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B08D756-EAC6-48C5-B791-6966BD5054FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F15074-CFAA-4445-A06F-B50DC452FBA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DAB1D4BE-B0C1-4C13-98F9-4212A95D167C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>partno</t>
   </si>
@@ -57,6 +57,15 @@
   </si>
   <si>
     <t>AL3KB0KARBOXSIKU5000</t>
+  </si>
+  <si>
+    <t>warehouse</t>
+  </si>
+  <si>
+    <t>whrm01</t>
+  </si>
+  <si>
+    <t>whrm02</t>
   </si>
 </sst>
 </file>
@@ -471,29 +480,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD6BD1A7-9674-4A48-858C-A767ED342D2D}">
-  <dimension ref="A2:AI17"/>
+  <dimension ref="A2:AJ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5:AI5"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="4.36328125" customWidth="1"/>
-    <col min="2" max="2" width="27.54296875" customWidth="1"/>
-    <col min="3" max="3" width="14.7265625" customWidth="1"/>
-    <col min="6" max="6" width="9.36328125" customWidth="1"/>
+    <col min="2" max="2" width="28.36328125" customWidth="1"/>
+    <col min="3" max="3" width="23.26953125" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" customWidth="1"/>
+    <col min="7" max="7" width="9.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -501,136 +512,139 @@
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="3">
         <v>1</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <v>2</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="3">
         <v>3</v>
       </c>
-      <c r="H3" s="3">
+      <c r="I3" s="3">
         <v>4</v>
       </c>
-      <c r="I3" s="3">
+      <c r="J3" s="3">
         <v>5</v>
       </c>
-      <c r="J3" s="3">
+      <c r="K3" s="3">
         <v>6</v>
       </c>
-      <c r="K3" s="3">
+      <c r="L3" s="3">
         <v>7</v>
       </c>
-      <c r="L3" s="3">
+      <c r="M3" s="3">
         <v>8</v>
       </c>
-      <c r="M3" s="3">
+      <c r="N3" s="3">
         <v>9</v>
       </c>
-      <c r="N3" s="3">
+      <c r="O3" s="3">
         <v>10</v>
       </c>
-      <c r="O3" s="3">
+      <c r="P3" s="3">
         <v>11</v>
       </c>
-      <c r="P3" s="3">
+      <c r="Q3" s="3">
         <v>12</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="R3" s="3">
         <v>13</v>
       </c>
-      <c r="R3" s="3">
+      <c r="S3" s="3">
         <v>14</v>
       </c>
-      <c r="S3" s="3">
+      <c r="T3" s="3">
         <v>15</v>
       </c>
-      <c r="T3" s="3">
+      <c r="U3" s="3">
         <v>16</v>
       </c>
-      <c r="U3" s="3">
+      <c r="V3" s="3">
         <v>17</v>
       </c>
-      <c r="V3" s="3">
+      <c r="W3" s="3">
         <v>18</v>
       </c>
-      <c r="W3" s="3">
+      <c r="X3" s="3">
         <v>19</v>
       </c>
-      <c r="X3" s="3">
+      <c r="Y3" s="3">
         <v>20</v>
       </c>
-      <c r="Y3" s="3">
+      <c r="Z3" s="3">
         <v>21</v>
       </c>
-      <c r="Z3" s="3">
+      <c r="AA3" s="3">
         <v>22</v>
       </c>
-      <c r="AA3" s="3">
+      <c r="AB3" s="3">
         <v>23</v>
       </c>
-      <c r="AB3" s="3">
+      <c r="AC3" s="3">
         <v>24</v>
       </c>
-      <c r="AC3" s="3">
+      <c r="AD3" s="3">
         <v>25</v>
       </c>
-      <c r="AD3" s="3">
+      <c r="AE3" s="3">
         <v>26</v>
       </c>
-      <c r="AE3" s="3">
+      <c r="AF3" s="3">
         <v>27</v>
       </c>
-      <c r="AF3" s="3">
+      <c r="AG3" s="3">
         <v>28</v>
       </c>
-      <c r="AG3" s="3">
+      <c r="AH3" s="3">
         <v>29</v>
       </c>
-      <c r="AH3" s="3">
+      <c r="AI3" s="3">
         <v>30</v>
       </c>
-      <c r="AI3" s="3">
+      <c r="AJ3" s="3">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3">
         <v>2026</v>
       </c>
-      <c r="D4" s="3">
+      <c r="E4" s="3">
         <v>1</v>
-      </c>
-      <c r="E4" s="3">
-        <v>300</v>
       </c>
       <c r="F4" s="3">
         <v>300</v>
       </c>
       <c r="G4" s="3">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
         <v>400</v>
       </c>
-      <c r="I4" s="3">
+      <c r="J4" s="3">
         <v>500</v>
       </c>
-      <c r="J4" s="3">
-        <v>0</v>
-      </c>
       <c r="K4" s="3">
         <v>0</v>
       </c>
@@ -706,38 +720,41 @@
       <c r="AI4" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3">
         <v>2026</v>
       </c>
-      <c r="D5" s="3">
+      <c r="E5" s="3">
         <v>1</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="3">
         <v>300</v>
       </c>
-      <c r="F5" s="3">
+      <c r="G5" s="3">
         <v>400</v>
       </c>
-      <c r="G5" s="3">
+      <c r="H5" s="3">
         <v>700</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="3">
         <v>900</v>
       </c>
-      <c r="I5" s="3">
+      <c r="J5" s="3">
         <v>100</v>
       </c>
-      <c r="J5" s="3">
-        <v>0</v>
-      </c>
       <c r="K5" s="3">
         <v>0</v>
       </c>
@@ -813,8 +830,11 @@
       <c r="AI5" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -852,8 +872,9 @@
       <c r="AG6" s="3"/>
       <c r="AH6" s="3"/>
       <c r="AI6" s="3"/>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ6" s="3"/>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -891,8 +912,9 @@
       <c r="AG7" s="3"/>
       <c r="AH7" s="3"/>
       <c r="AI7" s="3"/>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ7" s="3"/>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -930,8 +952,9 @@
       <c r="AG8" s="3"/>
       <c r="AH8" s="3"/>
       <c r="AI8" s="3"/>
-    </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ8" s="3"/>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -969,8 +992,9 @@
       <c r="AG9" s="3"/>
       <c r="AH9" s="3"/>
       <c r="AI9" s="3"/>
-    </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ9" s="3"/>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -1008,8 +1032,9 @@
       <c r="AG10" s="3"/>
       <c r="AH10" s="3"/>
       <c r="AI10" s="3"/>
-    </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ10" s="3"/>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -1047,8 +1072,9 @@
       <c r="AG11" s="3"/>
       <c r="AH11" s="3"/>
       <c r="AI11" s="3"/>
-    </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ11" s="3"/>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -1086,8 +1112,9 @@
       <c r="AG12" s="3"/>
       <c r="AH12" s="3"/>
       <c r="AI12" s="3"/>
-    </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ12" s="3"/>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -1125,30 +1152,35 @@
       <c r="AG13" s="3"/>
       <c r="AH13" s="3"/>
       <c r="AI13" s="3"/>
-    </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ13" s="3"/>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A2:E2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>